<commit_message>
ignore files in data; import in __init__; catch all exceptions in main(); update schema.xlsx and tests/fixtures/test_expense_data.xlsx for current obj_tables (1.0.13)
</commit_message>
<xml_diff>
--- a/summarize_expenses/schema.xlsx
+++ b/summarize_expenses/schema.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11500" yWindow="23420" windowWidth="14860" windowHeight="10800" tabRatio="500"/>
+    <workbookView xWindow="13920" yWindow="8300" windowWidth="11320" windowHeight="7700" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="!_Schema" sheetId="1" r:id="rId1"/>
+    <sheet name="!!_Schema" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,9 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
-    <t>!!ObjTables TableType='Schema' ObjTablesVersion='0.0.8'</t>
-  </si>
-  <si>
     <t>!Name</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>Payee</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
     <t>Attribute</t>
   </si>
   <si>
@@ -81,6 +75,12 @@
   </si>
   <si>
     <t>Float</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Schema' tableFormat='row'</t>
+  </si>
+  <si>
+    <t>Class</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -424,7 +424,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -433,103 +433,103 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>